<commit_message>
R: Bind-Methode_Refactoring begonnen. R: Ladefehler Dienstag gefixt
git-svn-id: svn://diskstation/Programmier%20Projekte@78 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0822759-AEDE-47C9-AF4A-13F07ECAD3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B4076E-EE1D-4FA8-8DFF-6B6EA3D618B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2730" windowWidth="20730" windowHeight="11835" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Scrollbar nach unten setzen.</t>
+  </si>
+  <si>
+    <t>Bind</t>
+  </si>
+  <si>
+    <t>Methode fertig recatoren</t>
   </si>
 </sst>
 </file>
@@ -562,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8623618-753D-47B9-9C0E-D7DB83973181}">
   <dimension ref="A1:K1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,6 +679,9 @@
       <c r="H3" s="1">
         <v>43945</v>
       </c>
+      <c r="I3" s="1">
+        <v>43947</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -813,9 +822,30 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="2" t="str">
+      <c r="A9" s="7">
+        <v>43945</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>43948</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Eigenschaftendialog: LoggingLevel hinzugefügt
git-svn-id: svn://diskstation/Programmier%20Projekte@80 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B4076E-EE1D-4FA8-8DFF-6B6EA3D618B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F29AA6-20B7-4B93-BCA2-C0C01F2C3F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2730" windowWidth="20730" windowHeight="11835" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
     <t>Bind</t>
   </si>
   <si>
-    <t>Methode fertig recatoren</t>
+    <t>Methode fertig refactoren</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8623618-753D-47B9-9C0E-D7DB83973181}">
   <dimension ref="A1:K1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,10 +842,13 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <v>43948</v>
+      </c>
+      <c r="J9" s="1">
+        <v>43946</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RR: Eigenschaften Fester Übersicht geändert
git-svn-id: svn://diskstation/Programmier%20Projekte@85 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmier Projekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3196345F-39F7-4313-A80C-593823EFE9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25442B18-D315-4D11-B983-71A0E07D63F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
+    <workbookView xWindow="5670" yWindow="2730" windowWidth="20910" windowHeight="13185" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Methode fertig refactoren</t>
+  </si>
+  <si>
+    <t>Eigenchaften Dialog</t>
+  </si>
+  <si>
+    <t>Für Logging Level erweitert</t>
   </si>
 </sst>
 </file>
@@ -569,7 +575,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,9 +864,30 @@
       <c r="A10" s="7">
         <v>43947</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43947</v>
+      </c>
+      <c r="J10" s="1">
+        <v>43947</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Neue Aufgabe für Filtern im Rezeptpool.
git-svn-id: svn://diskstation/Programmier%20Projekte@89 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmier Projekte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25442B18-D315-4D11-B983-71A0E07D63F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86195EE7-20A5-4999-967B-1737BCBAB97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="2730" windowWidth="20910" windowHeight="13185" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Für Logging Level erweitert</t>
+  </si>
+  <si>
+    <t>RezeptPool</t>
+  </si>
+  <si>
+    <t>Filtern nach Gericht implementieren</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,9 +900,27 @@
       <c r="A11" s="7">
         <v>43947</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>43949</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Filter in Rezeptauswahldialog.
git-svn-id: svn://diskstation/Programmier%20Projekte@91 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86195EE7-20A5-4999-967B-1737BCBAB97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF09BA-B099-48DA-99CF-17C0A68C1C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +917,13 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <v>43949</v>
+      </c>
+      <c r="J11" s="1">
+        <v>43947</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Neue Aufgaben hinzugefügt.
git-svn-id: svn://diskstation/Programmier%20Projekte@93 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF09BA-B099-48DA-99CF-17C0A68C1C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F1F76-94E0-47FC-A7B7-F20C3AD1149B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Filtern nach Gericht implementieren</t>
+  </si>
+  <si>
+    <t>Einheiten</t>
+  </si>
+  <si>
+    <t>In den Zutaten aus Auswahlbox (definiert im ini File)</t>
   </si>
 </sst>
 </file>
@@ -581,7 +587,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +698,7 @@
         <v>43945</v>
       </c>
       <c r="I3" s="1">
-        <v>43947</v>
+        <v>43949</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -927,9 +933,30 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G12" s="2" t="str">
+      <c r="A12" s="7">
+        <v>43947</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>43951</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Drucken der Einkaufsliste implementiert.
git-svn-id: svn://diskstation/Programmier%20Projekte@95 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F1F76-94E0-47FC-A7B7-F20C3AD1149B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD71554-BACE-4753-8E15-BC168783E859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>In den Zutaten aus Auswahlbox (definiert im ini File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speichern </t>
+  </si>
+  <si>
+    <t>zusätzlich zu Speichernunter implementieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unittest </t>
+  </si>
+  <si>
+    <t>für Berechnung der Einkaufsliste</t>
+  </si>
+  <si>
+    <t>Unittest</t>
+  </si>
+  <si>
+    <t>für Zutat.ToString();</t>
+  </si>
+  <si>
+    <t>Einkaufsliste</t>
+  </si>
+  <si>
+    <t>Man kann die Einkaufsliste editieren vor dem Drucken.</t>
   </si>
 </sst>
 </file>
@@ -587,7 +611,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,13 +716,16 @@
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G66" si="0">IF(E3="Aufgabe",IF(J3="",0,1),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1">
         <v>43945</v>
       </c>
       <c r="I3" s="1">
         <v>43949</v>
+      </c>
+      <c r="J3" s="1">
+        <v>43948</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -960,24 +987,102 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="2" t="str">
+      <c r="A13" s="7">
+        <v>43948</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>43951</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="2" t="str">
+      <c r="A14" s="7">
+        <v>43948</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>43951</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G15" s="2" t="str">
+      <c r="A15" s="7">
+        <v>43948</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>43951</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>43948</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
R: Interface für LoggingOutput. R: Unittest für Logging.
git-svn-id: svn://diskstation/Programmier%20Projekte@97 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD71554-BACE-4753-8E15-BC168783E859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8380CA0B-2AA2-4C95-AEBE-AE184FC46CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -176,6 +176,10 @@
   </si>
   <si>
     <t>Man kann die Einkaufsliste editieren vor dem Drucken.</t>
+  </si>
+  <si>
+    <t>Interface einziehen, damit Logging in Unittests getestet werden 
+kann.</t>
   </si>
 </sst>
 </file>
@@ -611,7 +615,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,10 +1038,13 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>43951</v>
+      </c>
+      <c r="J14" s="1">
+        <v>43949</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,10 +1068,13 @@
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
         <v>43951</v>
+      </c>
+      <c r="J15" s="1">
+        <v>43949</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1088,97 +1098,121 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="2" t="str">
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>43949</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>43949</v>
+      </c>
+      <c r="J17" s="1">
+        <v>43949</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
R: Singleton für IniFile und Logging
git-svn-id: svn://diskstation/Programmier%20Projekte@102 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmier Projekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD64AE7B-B97F-44BD-BDC1-7103C648BF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6C6282-EBE6-46F9-BC15-8611BF3B1C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -627,7 +627,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,9 +1161,12 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
+        <v>43954</v>
+      </c>
+      <c r="J18" s="1">
         <v>43954</v>
       </c>
     </row>
@@ -1188,9 +1191,12 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
+        <v>43954</v>
+      </c>
+      <c r="J19" s="1">
         <v>43954</v>
       </c>
     </row>

</xml_diff>

<commit_message>
R: Anzeige der Speicherpfades im Titel geschlossen.
git-svn-id: svn://diskstation/Programmier%20Projekte@113 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD909449-1780-4F45-8028-902DB251CBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD02CC-00FD-430D-9F92-33D3D621FA6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
   <si>
     <t>Datum</t>
   </si>
@@ -206,6 +206,15 @@
   <si>
     <t>Klasse Woche um Datum erweitern und das Datum auf der 
 Oberfläche anzeigen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominik </t>
+  </si>
+  <si>
+    <t>Dateiname</t>
+  </si>
+  <si>
+    <t>im Window anzeigen</t>
   </si>
 </sst>
 </file>
@@ -641,7 +650,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,12 +878,15 @@
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
         <v>43951</v>
       </c>
       <c r="I7" s="1">
+        <v>43959</v>
+      </c>
+      <c r="J7" s="1">
         <v>43959</v>
       </c>
     </row>
@@ -1287,9 +1299,33 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="2" t="str">
+      <c r="A22" s="7">
+        <v>43959</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>43961</v>
+      </c>
+      <c r="J22" s="1">
+        <v>43959</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
R: Rechtschribprüfung R: Tests für Load  / Save
git-svn-id: svn://diskstation/Programmier%20Projekte@132 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD02CC-00FD-430D-9F92-33D3D621FA6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCA6A2C-1783-4A9E-AA18-35C7D01ACF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="63">
   <si>
     <t>Datum</t>
   </si>
@@ -215,6 +215,22 @@
   </si>
   <si>
     <t>im Window anzeigen</t>
+  </si>
+  <si>
+    <t>als File speichern</t>
+  </si>
+  <si>
+    <t>Eine neue Methode in der Klasse Logging.
+Speichern als .txt file</t>
+  </si>
+  <si>
+    <t>Rechtschreibung</t>
+  </si>
+  <si>
+    <t>prüfen auch in den anderen Tagen ausser Montag</t>
+  </si>
+  <si>
+    <t>Im Montag XAML Code sieht man wie es geht.</t>
   </si>
 </sst>
 </file>
@@ -650,7 +666,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1167,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43949</v>
       </c>
@@ -1181,7 +1197,7 @@
         <v>43949</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43954</v>
       </c>
@@ -1211,7 +1227,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>43954</v>
       </c>
@@ -1241,7 +1257,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>43955</v>
       </c>
@@ -1271,7 +1287,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43955</v>
       </c>
@@ -1298,7 +1314,7 @@
         <v>43960</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>43959</v>
       </c>
@@ -1328,61 +1344,109 @@
         <v>43959</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="2" t="str">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>43966</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>43971</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>43966</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>43967</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
R: Spaltenbreite in Rezeptliste automatisch.
git-svn-id: svn://diskstation/Programmier%20Projekte@138 9a2fd316-128d-4348-9d11-99372ba87f9e
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daten Klaus\SVN Working Copies Programmierprojekte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCA6A2C-1783-4A9E-AA18-35C7D01ACF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E80127-D9C9-495F-B09B-24072E4F7E4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{3D802DA4-F663-4471-B7D6-A3476ECFC0E4}"/>
   </bookViews>
@@ -666,7 +666,7 @@
   <dimension ref="A1:K1500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43943</v>
       </c>
@@ -810,7 +810,7 @@
         <v>43949</v>
       </c>
       <c r="I4" s="1">
-        <v>43959</v>
+        <v>43981</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>43949</v>
       </c>
       <c r="I5" s="1">
-        <v>43959</v>
+        <v>43981</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>43951</v>
       </c>
       <c r="I12" s="1">
-        <v>43959</v>
+        <v>43981</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="1">
-        <v>43960</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1395,16 +1395,22 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1">
         <v>43967</v>
       </c>
+      <c r="J24" s="1">
+        <v>43967</v>
+      </c>
       <c r="K24" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>43975</v>
+      </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>